<commit_message>
[modify]rakuten,yahoo iframe and explanation
</commit_message>
<xml_diff>
--- a/readme/tasklist.xlsx
+++ b/readme/tasklist.xlsx
@@ -2146,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2674,9 +2674,11 @@
       <c r="D30" s="66"/>
       <c r="E30" s="67"/>
       <c r="F30" s="68"/>
-      <c r="G30" s="13"/>
+      <c r="G30" s="13">
+        <v>42032</v>
+      </c>
       <c r="H30" s="12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>74</v>
@@ -2689,9 +2691,7 @@
       <c r="D31" s="64"/>
       <c r="E31" s="40"/>
       <c r="F31" s="12"/>
-      <c r="G31" s="13">
-        <v>42022</v>
-      </c>
+      <c r="G31" s="13"/>
       <c r="H31" s="12" t="s">
         <v>16</v>
       </c>

</xml_diff>